<commit_message>
add status in rm and pt
</commit_message>
<xml_diff>
--- a/BMI/wwwroot/Uploads/GI.xlsx
+++ b/BMI/wwwroot/Uploads/GI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frizal\OneDrive - bumblebeeseafoods\Documents\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2810BD-A901-4C9B-BE4B-520399253E97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2B88C7-58D7-4B10-B06A-D517903AD847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GI" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -77,7 +77,7 @@
     <t>rm_sources</t>
   </si>
   <si>
-    <t>09112SIDID</t>
+    <t>09113SIDID</t>
   </si>
 </sst>
 </file>
@@ -919,17 +919,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -968,7 +968,7 @@
         <v>44055</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -994,7 +994,7 @@
         <v>44055</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1020,7 +1020,7 @@
         <v>44055</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1046,7 +1046,7 @@
         <v>44055</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -1061,6 +1061,110 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6800083954</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44056</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6800083955</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44056</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>390</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6800083955</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44056</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>5580</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6800083955</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44056</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>1230</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>